<commit_message>
Confirmed with Jill that no P levels should be included but M1 should be, updated and re ran the code before sending out.
</commit_message>
<xml_diff>
--- a/outputs/Internal Fill Data Validation.xlsx
+++ b/outputs/Internal Fill Data Validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://regalrexnord-my.sharepoint.com/personal/jenna_eagleson_regalrexnord_com/Documents/Documents/2024/2024_Core Value Drivers_Reporting/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_3E5C2B06141573791A626765304942E08E99AB8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A2AB1A9-17A7-4186-A167-073815A32E35}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_3E5C2B066FCD3325A2E36365304942E08E999DBA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58D625DF-E2F9-464B-8E36-6D5BE7408363}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Profile No Move" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
   <si>
     <t>employee_id</t>
   </si>
@@ -108,33 +108,6 @@
     <t>Molndal Sweden</t>
   </si>
   <si>
-    <t>610159455</t>
-  </si>
-  <si>
-    <t>Henok Mezgebe Fanta</t>
-  </si>
-  <si>
-    <t>Industrial Powertrain Solutions (IPS)</t>
-  </si>
-  <si>
-    <t>IPS Clutches &amp; Brakes Division</t>
-  </si>
-  <si>
-    <t>Bedford United Kingdom</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>220654845</t>
-  </si>
-  <si>
-    <t>Anja Bruns</t>
-  </si>
-  <si>
-    <t>Unna Germany</t>
-  </si>
-  <si>
     <t>610169796</t>
   </si>
   <si>
@@ -150,54 +123,27 @@
     <t>M5</t>
   </si>
   <si>
-    <t>100003792</t>
-  </si>
-  <si>
-    <t>Alejandro Vargas Cruz</t>
+    <t>501012633</t>
+  </si>
+  <si>
+    <t>Paul Boyer</t>
   </si>
   <si>
     <t>PES NA Motors and Drives</t>
   </si>
   <si>
-    <t>Monterrey Rbm Mexico</t>
-  </si>
-  <si>
-    <t>501012633</t>
-  </si>
-  <si>
-    <t>Paul Boyer</t>
-  </si>
-  <si>
     <t>Fort Wayne Indiana</t>
   </si>
   <si>
-    <t>610062783</t>
-  </si>
-  <si>
-    <t>Alma Estefania Cortes Aguilar</t>
-  </si>
-  <si>
-    <t>100001745</t>
-  </si>
-  <si>
-    <t>Tom Faxlanger</t>
+    <t>100002185</t>
+  </si>
+  <si>
+    <t>Matthew Miller</t>
   </si>
   <si>
     <t>PES NA Sales</t>
   </si>
   <si>
-    <t>100002185</t>
-  </si>
-  <si>
-    <t>Matthew Miller</t>
-  </si>
-  <si>
-    <t>610067977</t>
-  </si>
-  <si>
-    <t>Troy Hankins</t>
-  </si>
-  <si>
     <t>610125381</t>
   </si>
   <si>
@@ -213,18 +159,6 @@
     <t>Bob Doenges</t>
   </si>
   <si>
-    <t>610135945</t>
-  </si>
-  <si>
-    <t>Greg Lees</t>
-  </si>
-  <si>
-    <t>610146150</t>
-  </si>
-  <si>
-    <t>Marcus Peters</t>
-  </si>
-  <si>
     <t>220138520</t>
   </si>
   <si>
@@ -264,6 +198,21 @@
     <t>Apodaca Pmc Plant 2 Mexico</t>
   </si>
   <si>
+    <t>610158896</t>
+  </si>
+  <si>
+    <t>Frank Miller</t>
+  </si>
+  <si>
+    <t>AMC Linear Motion Division</t>
+  </si>
+  <si>
+    <t>East Aurora New York</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
     <t>220261238</t>
   </si>
   <si>
@@ -301,9 +250,6 @@
   </si>
   <si>
     <t>hris_response</t>
-  </si>
-  <si>
-    <t>hris_responder</t>
   </si>
 </sst>
 </file>
@@ -663,11 +609,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -797,7 +741,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="2">
-        <v>45341</v>
+        <v>45600</v>
       </c>
       <c r="D4" s="2">
         <v>45658</v>
@@ -806,45 +750,45 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
         <v>30</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>32</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
       <c r="C5" s="2">
-        <v>45013</v>
+        <v>35379</v>
       </c>
       <c r="D5" s="2">
-        <v>45658</v>
+        <v>45662</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -855,10 +799,10 @@
         <v>38</v>
       </c>
       <c r="C6" s="2">
-        <v>45600</v>
+        <v>38782</v>
       </c>
       <c r="D6" s="2">
-        <v>45658</v>
+        <v>45663</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -870,24 +814,24 @@
         <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2">
-        <v>43640</v>
+        <v>44249</v>
       </c>
       <c r="D7" s="2">
-        <v>45662</v>
+        <v>45663</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -896,27 +840,27 @@
         <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2">
-        <v>35379</v>
+        <v>44306</v>
       </c>
       <c r="D8" s="2">
-        <v>45662</v>
+        <v>45663</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -925,10 +869,10 @@
         <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
@@ -936,31 +880,31 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" s="2">
-        <v>43640</v>
+        <v>39343</v>
       </c>
       <c r="D9" s="2">
-        <v>45662</v>
+        <v>45667</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -971,25 +915,25 @@
         <v>52</v>
       </c>
       <c r="C10" s="2">
-        <v>34659</v>
+        <v>42961</v>
       </c>
       <c r="D10" s="2">
-        <v>45663</v>
+        <v>45670</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
         <v>53</v>
       </c>
-      <c r="H10" t="s">
-        <v>48</v>
-      </c>
       <c r="I10" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
@@ -1000,286 +944,83 @@
         <v>55</v>
       </c>
       <c r="C11" s="2">
-        <v>38782</v>
+        <v>44608</v>
       </c>
       <c r="D11" s="2">
-        <v>45663</v>
+        <v>45684</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2">
-        <v>42373</v>
+        <v>45250</v>
       </c>
       <c r="D12" s="2">
-        <v>45663</v>
+        <v>45684</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2">
-        <v>44249</v>
+        <v>45688</v>
       </c>
       <c r="D13" s="2">
-        <v>45663</v>
+        <v>45688</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="I13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="2">
-        <v>44306</v>
-      </c>
-      <c r="D14" s="2">
-        <v>45663</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" t="s">
-        <v>48</v>
-      </c>
-      <c r="I14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="2">
-        <v>44515</v>
-      </c>
-      <c r="D15" s="2">
-        <v>45663</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" t="s">
         <v>66</v>
-      </c>
-      <c r="C16" s="2">
-        <v>44851</v>
-      </c>
-      <c r="D16" s="2">
-        <v>45663</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="2">
-        <v>39343</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45667</v>
-      </c>
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" t="s">
-        <v>71</v>
-      </c>
-      <c r="I17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="2">
-        <v>42961</v>
-      </c>
-      <c r="D18" s="2">
-        <v>45670</v>
-      </c>
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" t="s">
-        <v>75</v>
-      </c>
-      <c r="I18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="2">
-        <v>44608</v>
-      </c>
-      <c r="D19" s="2">
-        <v>45684</v>
-      </c>
-      <c r="E19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" t="s">
-        <v>79</v>
-      </c>
-      <c r="I19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="2">
-        <v>45688</v>
-      </c>
-      <c r="D20" s="2">
-        <v>45688</v>
-      </c>
-      <c r="E20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1291,9 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1343,40 +1082,40 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="E2" s="3">
         <v>45658</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="L2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1385,36 +1124,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2358A7A5-6533-43B0-BA41-026DAC272B81}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E255C95D-9A16-444C-97E7-34A65EB7506E}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Okay, for realz this time, this is the version being shared
</commit_message>
<xml_diff>
--- a/outputs/Internal Fill Data Validation.xlsx
+++ b/outputs/Internal Fill Data Validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://regalrexnord-my.sharepoint.com/personal/jenna_eagleson_regalrexnord_com/Documents/Documents/2024/2024_Core Value Drivers_Reporting/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_3E5C2B066FCD3325A2E36365304942E08E999DBA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58D625DF-E2F9-464B-8E36-6D5BE7408363}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_3E5C2B066F0D335E72A17165304942E08E999DBA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1DA37E5-BE97-42A0-98C2-2ACB79545E98}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Profile No Move" sheetId="1" r:id="rId1"/>
@@ -1124,19 +1124,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E255C95D-9A16-444C-97E7-34A65EB7506E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239D7947-E4A1-46A0-AC5C-755429E334C8}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added more dcoumentation throughout file
</commit_message>
<xml_diff>
--- a/outputs/Internal Fill Data Validation.xlsx
+++ b/outputs/Internal Fill Data Validation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28605"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -17,7 +17,23 @@
     <sheet name="Promo or Lateral No New Profile" sheetId="2" r:id="rId2"/>
     <sheet name="Flags" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -260,7 +276,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,13 +629,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="3" max="4" width="20.7265625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="20.7265625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -704,7 +720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -733,7 +749,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -762,7 +778,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -791,7 +807,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -820,7 +836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -849,7 +865,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -878,7 +894,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -907,7 +923,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -936,7 +952,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -965,7 +981,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -994,7 +1010,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -1034,12 +1050,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="5" max="5" width="20.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1096,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1131,15 +1147,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>